<commit_message>
Preview site content update
</commit_message>
<xml_diff>
--- a/content/species/data/sp_am_table2.xlsx
+++ b/content/species/data/sp_am_table2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Maphale Monyeki Projects\NBA 2025\2. NBA 2025 - Modules\species\quarto\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Maphale Monyeki Projects\NBA 2025\2. NBA 2025 - Modules\2. Modules\species\quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A49E8D26-9492-4AD5-8B7C-CC750E93FD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5341F279-DA9F-4E5A-9309-921714E62275}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="0" windowWidth="12276" windowHeight="12240" xr2:uid="{94A7674F-F120-4B77-A9BA-5E660C67A06B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14892" windowHeight="12240" xr2:uid="{94A7674F-F120-4B77-A9BA-5E660C67A06B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Taxon</t>
   </si>
@@ -62,22 +62,13 @@
     <t>Increase </t>
   </si>
   <si>
-    <t>Based on the projected increased threats from mining and development. New information on future threatening processes has become available with changes in government policy that will likely lead to increased industrial development in the coastal region of the Northern Cape, South Africa and southwestern Namibia. </t>
-  </si>
-  <si>
-    <t>[*Hyperolius poweri*]\* (https://www.inaturalist.org/observations?place_id=6986&amp;preferred_place_id=6986&amp;taxon_id=65730)</t>
-  </si>
-  <si>
-    <t>LC to NT </t>
-  </si>
-  <si>
-    <t>Large extents of this species range are impacted by habitat loss and degradation caused by urban coastal development, mining, afforestation, and agriculture (especially sugar cane plantations), which have caused wetland drainage and degradation through trampling from cattle. Over 85% of the species’ known range occurs outside of protected areas and it occurs in a region of heavy development pressure. </t>
-  </si>
-  <si>
-    <t>Deterioration in habitat quality, especially in Lesotho where mines and proposed mines have had an observable increased impact (both directly and indirectly) on this species, with projected increased aridification due to climate change, and overgrazing and water quality issues that have intensified since the last assessment, resulting in this species’ conservation status deteriorating.</t>
-  </si>
-  <si>
     <t>[*Amietia hymenopus*]\** (https://www.inaturalist.org/observations?verifiable=true&amp;taxon_id=476398&amp;place_id=6986&amp;preferred_place_id=6986)</t>
+  </si>
+  <si>
+    <t>Deterioration in habitat quality, especially in Lesotho where active and proposed mines  have had an observable increased impact (both directly and indirectly) on this species, with projected increased aridification due to climate change, overgrazing and water quality issues that have intensified since the last assessment, resulting in this species’ conservation status deteriorating.</t>
+  </si>
+  <si>
+    <t>Based on projected increased threats from mining and development. New information on future threatening processes has become available with changes in government policy that will likely lead to increased industrial development in the coastal region of the Northern Cape, South Africa and southwestern Namibia.</t>
   </si>
 </sst>
 </file>
@@ -500,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9916F188-DE88-4CAE-98C2-703B4DE9398E}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -530,7 +521,7 @@
     </row>
     <row r="2" spans="1:4" ht="201.6">
       <c r="A2" s="8" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>4</v>
@@ -539,10 +530,10 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="172.8">
+    <row r="3" spans="1:4" ht="158.4">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -553,21 +544,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="201.6">
-      <c r="A4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -585,6 +562,19 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d08e37f2-beba-4595-a3e8-aa91f032b3fc" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de6781d5-cbdf-44cc-b8b1-919d4413b058">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A9251B87A2689245AA9FD86C69F20C58" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3a4ec884e7468e8b6decba7ff9ee350d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="de6781d5-cbdf-44cc-b8b1-919d4413b058" xmlns:ns3="d08e37f2-beba-4595-a3e8-aa91f032b3fc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b02cf9d369237c4b82eaa1e33230624f" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -856,19 +846,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d08e37f2-beba-4595-a3e8-aa91f032b3fc" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="de6781d5-cbdf-44cc-b8b1-919d4413b058">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8217B55-E0DA-4004-B599-CB3442C8A9D5}">
   <ds:schemaRefs>
@@ -878,6 +855,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A5A410E-81CD-4706-8086-DF1C2D66F289}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d08e37f2-beba-4595-a3e8-aa91f032b3fc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="de6781d5-cbdf-44cc-b8b1-919d4413b058"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C5385B4-FC77-4158-A42F-8D4135992DEB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -895,16 +884,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A5A410E-81CD-4706-8086-DF1C2D66F289}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d08e37f2-beba-4595-a3e8-aa91f032b3fc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="de6781d5-cbdf-44cc-b8b1-919d4413b058"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>